<commit_message>
+ prayer worker add
</commit_message>
<xml_diff>
--- a/public/spreadsheets/versiculo-exemplo.xlsx
+++ b/public/spreadsheets/versiculo-exemplo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>content</t>
   </si>
@@ -22,10 +22,16 @@
     <t>createdAt</t>
   </si>
   <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
     <t>Meu Versiculo 1</t>
   </si>
   <si>
     <t>VE 1:1</t>
+  </si>
+  <si>
+    <t>https://ranetium.com/favicon.ico</t>
   </si>
   <si>
     <t>Meu Versiculo 2</t>
@@ -47,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -58,6 +64,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,7 +84,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -82,6 +92,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -299,6 +312,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="24.38"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -310,41 +326,58 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>45888.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>45889.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>45890.0</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D3"/>
+    <hyperlink r:id="rId3" ref="D4"/>
+  </hyperlinks>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>